<commit_message>
einfügen in excel datei, bitte ändere den pfad bei dir, thx
</commit_message>
<xml_diff>
--- a/keto.xlsx
+++ b/keto.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\Tasnim\keto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106EB0B2-14A7-44F6-8B18-6BB924EE0569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A57C4BF-DE2C-4EC8-A370-8D81ABB2CC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{156E273D-FF48-495A-B4EE-4E91FE152371}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="118">
   <si>
     <t>menge</t>
   </si>
@@ -366,6 +366,30 @@
   </si>
   <si>
     <t>Aubergine</t>
+  </si>
+  <si>
+    <t>haselnusskerne</t>
+  </si>
+  <si>
+    <t>68.4</t>
+  </si>
+  <si>
+    <t>5.6</t>
+  </si>
+  <si>
+    <t>16.3</t>
+  </si>
+  <si>
+    <t>mandelnkerne</t>
+  </si>
+  <si>
+    <t>53.3</t>
+  </si>
+  <si>
+    <t>4.8</t>
+  </si>
+  <si>
+    <t>24.5</t>
   </si>
 </sst>
 </file>
@@ -737,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74DDAA16-A6EC-458B-A865-01F86C1E3CCF}">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A39" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1745,6 +1769,46 @@
         <v>17</v>
       </c>
     </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>110</v>
+      </c>
+      <c r="B51">
+        <v>100</v>
+      </c>
+      <c r="C51" t="s">
+        <v>111</v>
+      </c>
+      <c r="D51" t="s">
+        <v>112</v>
+      </c>
+      <c r="E51" t="s">
+        <v>113</v>
+      </c>
+      <c r="F51">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>114</v>
+      </c>
+      <c r="B52">
+        <v>100</v>
+      </c>
+      <c r="C52" t="s">
+        <v>115</v>
+      </c>
+      <c r="D52" t="s">
+        <v>116</v>
+      </c>
+      <c r="E52" t="s">
+        <v>117</v>
+      </c>
+      <c r="F52">
+        <v>621</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
neue art von essen, süßigkeiten
</commit_message>
<xml_diff>
--- a/keto.xlsx
+++ b/keto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\Tasnim\keto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C379E08-2953-48BE-B7D0-4200CAA2A3A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA72A31-82A9-4984-A4D3-306E59FE0D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{156E273D-FF48-495A-B4EE-4E91FE152371}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="135">
   <si>
     <t>menge</t>
   </si>
@@ -185,12 +185,6 @@
     <t>15.5</t>
   </si>
   <si>
-    <t>52.4</t>
-  </si>
-  <si>
-    <t>20.8</t>
-  </si>
-  <si>
     <t>6.7</t>
   </si>
   <si>
@@ -218,18 +212,12 @@
     <t>fat</t>
   </si>
   <si>
-    <t>100.1</t>
-  </si>
-  <si>
     <t>egg</t>
   </si>
   <si>
     <t>butter</t>
   </si>
   <si>
-    <t>almond</t>
-  </si>
-  <si>
     <t>avocado</t>
   </si>
   <si>
@@ -329,9 +317,6 @@
     <t>23.5</t>
   </si>
   <si>
-    <t>haselnusskerne</t>
-  </si>
-  <si>
     <t>68.4</t>
   </si>
   <si>
@@ -431,9 +416,6 @@
     <t>chicken_wings</t>
   </si>
   <si>
-    <t>rind_Rippe/hals</t>
-  </si>
-  <si>
     <t>gehackte_tomaten</t>
   </si>
   <si>
@@ -444,6 +426,21 @@
   </si>
   <si>
     <t>aubergine</t>
+  </si>
+  <si>
+    <t>garnelen</t>
+  </si>
+  <si>
+    <t>haselnuss_kerne</t>
+  </si>
+  <si>
+    <t>rind_rippe/hals</t>
+  </si>
+  <si>
+    <t>gemahlen_mandeln</t>
+  </si>
+  <si>
+    <t>griechischer_joghurt</t>
   </si>
 </sst>
 </file>
@@ -815,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74DDAA16-A6EC-458B-A865-01F86C1E3CCF}">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -828,13 +825,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -860,7 +857,7 @@
         <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F2">
         <v>26</v>
@@ -868,7 +865,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -908,7 +905,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B5">
         <v>100</v>
@@ -948,7 +945,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B7">
         <v>100</v>
@@ -968,7 +965,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B8">
         <v>100</v>
@@ -988,7 +985,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B9">
         <v>100</v>
@@ -1048,7 +1045,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B12">
         <v>100</v>
@@ -1068,7 +1065,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B13">
         <v>100</v>
@@ -1088,7 +1085,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B14">
         <v>100</v>
@@ -1148,7 +1145,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B17">
         <v>114</v>
@@ -1168,7 +1165,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B18">
         <v>119</v>
@@ -1306,29 +1303,9 @@
         <v>650</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25">
-        <v>593</v>
-      </c>
-    </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B26">
         <v>100</v>
@@ -1340,7 +1317,7 @@
         <v>33</v>
       </c>
       <c r="E26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F26">
         <v>635</v>
@@ -1348,7 +1325,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B27">
         <v>100</v>
@@ -1368,7 +1345,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B28">
         <v>100</v>
@@ -1388,7 +1365,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B29">
         <v>100</v>
@@ -1400,7 +1377,7 @@
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F29">
         <v>256</v>
@@ -1408,7 +1385,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B30">
         <v>108</v>
@@ -1428,16 +1405,16 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B31">
         <v>100</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E31">
         <v>2</v>
@@ -1448,7 +1425,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B32">
         <v>100</v>
@@ -1457,7 +1434,7 @@
         <v>25</v>
       </c>
       <c r="D32" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E32" t="s">
         <v>29</v>
@@ -1468,7 +1445,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B33">
         <v>100</v>
@@ -1477,7 +1454,7 @@
         <v>77</v>
       </c>
       <c r="D33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E33">
         <v>9</v>
@@ -1488,7 +1465,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B34">
         <v>100</v>
@@ -1497,7 +1474,7 @@
         <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E34">
         <v>22</v>
@@ -1508,7 +1485,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B35">
         <v>100</v>
@@ -1525,7 +1502,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B36">
         <v>100</v>
@@ -1545,13 +1522,13 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B37">
         <v>100</v>
       </c>
       <c r="C37" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D37" t="s">
         <v>6</v>
@@ -1565,7 +1542,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B38">
         <v>100</v>
@@ -1574,10 +1551,10 @@
         <v>32</v>
       </c>
       <c r="D38" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E38" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F38">
         <v>20</v>
@@ -1585,7 +1562,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B39">
         <v>100</v>
@@ -1594,7 +1571,7 @@
         <v>32</v>
       </c>
       <c r="D39" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -1605,13 +1582,13 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B40">
         <v>100</v>
       </c>
       <c r="C40" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D40" t="s">
         <v>14</v>
@@ -1625,7 +1602,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B41">
         <v>100</v>
@@ -1645,7 +1622,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B42">
         <v>100</v>
@@ -1657,7 +1634,7 @@
         <v>9</v>
       </c>
       <c r="E42" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F42">
         <v>29</v>
@@ -1665,19 +1642,19 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B43">
         <v>100</v>
       </c>
       <c r="C43" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D43" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E43" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F43">
         <v>53</v>
@@ -1685,7 +1662,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B44">
         <v>100</v>
@@ -1705,7 +1682,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B45">
         <v>100</v>
@@ -1725,7 +1702,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B46">
         <v>100</v>
@@ -1737,7 +1714,7 @@
         <v>2</v>
       </c>
       <c r="E46" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F46">
         <v>18</v>
@@ -1745,7 +1722,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B47">
         <v>100</v>
@@ -1765,7 +1742,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B48">
         <v>100</v>
@@ -1785,7 +1762,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B49">
         <v>100</v>
@@ -1797,7 +1774,7 @@
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F49">
         <v>323</v>
@@ -1805,7 +1782,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B50">
         <v>100</v>
@@ -1825,19 +1802,19 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>97</v>
+        <v>131</v>
       </c>
       <c r="B51">
         <v>100</v>
       </c>
       <c r="C51" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D51" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E51" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F51">
         <v>716</v>
@@ -1845,19 +1822,19 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B52">
         <v>100</v>
       </c>
       <c r="C52" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D52" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E52" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F52">
         <v>621</v>
@@ -1865,16 +1842,16 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B53">
         <v>100</v>
       </c>
       <c r="C53" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D53" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E53">
         <v>30</v>
@@ -1885,13 +1862,13 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B54">
         <v>100</v>
       </c>
       <c r="C54" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D54">
         <v>4</v>
@@ -1905,13 +1882,13 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B55">
         <v>100</v>
       </c>
       <c r="C55" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -1925,7 +1902,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B56">
         <v>100</v>
@@ -1945,7 +1922,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B57">
         <v>100</v>
@@ -1965,7 +1942,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B58">
         <v>100</v>
@@ -1974,10 +1951,10 @@
         <v>37</v>
       </c>
       <c r="D58" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E58" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F58">
         <v>364</v>
@@ -1985,13 +1962,13 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B59">
         <v>100</v>
       </c>
       <c r="C59" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D59">
         <v>3</v>
@@ -2005,7 +1982,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B60">
         <v>100</v>
@@ -2014,10 +1991,10 @@
         <v>23</v>
       </c>
       <c r="D60" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E60" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F60">
         <v>87</v>
@@ -2025,7 +2002,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B61">
         <v>100</v>
@@ -2034,13 +2011,93 @@
         <v>14</v>
       </c>
       <c r="D61" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E61" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F61">
         <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>130</v>
+      </c>
+      <c r="B62">
+        <v>100</v>
+      </c>
+      <c r="C62" t="s">
+        <v>26</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>14</v>
+      </c>
+      <c r="F62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>117</v>
+      </c>
+      <c r="B63">
+        <v>100</v>
+      </c>
+      <c r="C63">
+        <v>92</v>
+      </c>
+      <c r="D63" t="s">
+        <v>14</v>
+      </c>
+      <c r="E63" t="s">
+        <v>14</v>
+      </c>
+      <c r="F63">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>133</v>
+      </c>
+      <c r="B64">
+        <v>100</v>
+      </c>
+      <c r="C64">
+        <v>53</v>
+      </c>
+      <c r="D64" t="s">
+        <v>108</v>
+      </c>
+      <c r="E64">
+        <v>24</v>
+      </c>
+      <c r="F64">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>134</v>
+      </c>
+      <c r="B65">
+        <v>100</v>
+      </c>
+      <c r="C65">
+        <v>10</v>
+      </c>
+      <c r="D65" t="s">
+        <v>75</v>
+      </c>
+      <c r="E65" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>